<commit_message>
Updated Gantt chart 10-7
</commit_message>
<xml_diff>
--- a/Planning/Felzan_Gantt.xlsx
+++ b/Planning/Felzan_Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDDA981-0232-0F4C-B141-ED5DEA79375D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717DB8E2-16C1-F542-99EA-21254D8F0E74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1369,6 +1369,21 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="31" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1376,21 +1391,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1407,37 +1407,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1594,15 +1564,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstColumn" dxfId="14"/>
-      <tableStyleElement type="lastColumn" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="lastColumn" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2021,8 +1991,8 @@
   <dimension ref="A1:BL33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="97" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z5" sqref="Z5"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2073,117 +2043,117 @@
       <c r="B3" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="127">
+      <c r="D3" s="127"/>
+      <c r="E3" s="124">
         <v>44452</v>
       </c>
-      <c r="F3" s="128"/>
+      <c r="F3" s="125"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="122"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="124">
+      <c r="I4" s="121">
         <f>I5</f>
         <v>44452</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="124">
+      <c r="J4" s="122"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="122"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="121">
         <f>P5</f>
         <v>44459</v>
       </c>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="124">
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="121">
         <f>W5</f>
         <v>44466</v>
       </c>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AB4" s="125"/>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="124">
+      <c r="X4" s="122"/>
+      <c r="Y4" s="122"/>
+      <c r="Z4" s="122"/>
+      <c r="AA4" s="122"/>
+      <c r="AB4" s="122"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="121">
         <f>AD5</f>
         <v>44473</v>
       </c>
-      <c r="AE4" s="125"/>
-      <c r="AF4" s="125"/>
-      <c r="AG4" s="125"/>
-      <c r="AH4" s="125"/>
-      <c r="AI4" s="125"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="124">
+      <c r="AE4" s="122"/>
+      <c r="AF4" s="122"/>
+      <c r="AG4" s="122"/>
+      <c r="AH4" s="122"/>
+      <c r="AI4" s="122"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="121">
         <f>AK5</f>
         <v>44480</v>
       </c>
-      <c r="AL4" s="125"/>
-      <c r="AM4" s="125"/>
-      <c r="AN4" s="125"/>
-      <c r="AO4" s="125"/>
-      <c r="AP4" s="125"/>
-      <c r="AQ4" s="126"/>
-      <c r="AR4" s="124">
+      <c r="AL4" s="122"/>
+      <c r="AM4" s="122"/>
+      <c r="AN4" s="122"/>
+      <c r="AO4" s="122"/>
+      <c r="AP4" s="122"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="121">
         <f>AR5</f>
         <v>44487</v>
       </c>
-      <c r="AS4" s="125"/>
-      <c r="AT4" s="125"/>
-      <c r="AU4" s="125"/>
-      <c r="AV4" s="125"/>
-      <c r="AW4" s="125"/>
-      <c r="AX4" s="126"/>
-      <c r="AY4" s="124">
+      <c r="AS4" s="122"/>
+      <c r="AT4" s="122"/>
+      <c r="AU4" s="122"/>
+      <c r="AV4" s="122"/>
+      <c r="AW4" s="122"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="121">
         <f>AY5</f>
         <v>44494</v>
       </c>
-      <c r="AZ4" s="125"/>
-      <c r="BA4" s="125"/>
-      <c r="BB4" s="125"/>
-      <c r="BC4" s="125"/>
-      <c r="BD4" s="125"/>
-      <c r="BE4" s="126"/>
-      <c r="BF4" s="124">
+      <c r="AZ4" s="122"/>
+      <c r="BA4" s="122"/>
+      <c r="BB4" s="122"/>
+      <c r="BC4" s="122"/>
+      <c r="BD4" s="122"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="121">
         <f>BF5</f>
         <v>44501</v>
       </c>
-      <c r="BG4" s="125"/>
-      <c r="BH4" s="125"/>
-      <c r="BI4" s="125"/>
-      <c r="BJ4" s="125"/>
-      <c r="BK4" s="125"/>
-      <c r="BL4" s="126"/>
+      <c r="BG4" s="122"/>
+      <c r="BH4" s="122"/>
+      <c r="BI4" s="122"/>
+      <c r="BJ4" s="122"/>
+      <c r="BK4" s="122"/>
+      <c r="BL4" s="123"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44452</v>
@@ -2972,7 +2942,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="35">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E11" s="38">
         <f>F10</f>
@@ -3134,7 +3104,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="35">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E13" s="38">
         <f>F11</f>
@@ -3215,7 +3185,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="101">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E14" s="41">
         <f>F13</f>
@@ -4767,6 +4737,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4774,11 +4749,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D11 D13:D28">
     <cfRule type="dataBar" priority="26">
@@ -4795,15 +4765,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL11 I13:BL33">
-    <cfRule type="expression" dxfId="8" priority="45">
+    <cfRule type="expression" dxfId="5" priority="45">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL11 I13:BL33">
-    <cfRule type="expression" dxfId="7" priority="39">
+    <cfRule type="expression" dxfId="4" priority="39">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="40" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added final paper, final notebook, all background research articles
</commit_message>
<xml_diff>
--- a/Planning/Felzan_Gantt.xlsx
+++ b/Planning/Felzan_Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10339EEB-9AB9-3F46-AF28-0B2DED4309A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDAFA7F-48F4-4F4A-9897-315BD85CFA69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>Project Start:</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Decide on swath of spatial analysis/interpolation tools that would be reasonable with dataset/problem at hand</t>
+  </si>
+  <si>
+    <t>(aborted)</t>
+  </si>
+  <si>
+    <t>(aborted for now)</t>
   </si>
 </sst>
 </file>
@@ -1369,6 +1375,21 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="31" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1376,21 +1397,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1991,8 +1997,8 @@
   <dimension ref="A1:BL33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="97" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2043,117 +2049,117 @@
       <c r="B3" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="127">
+      <c r="D3" s="127"/>
+      <c r="E3" s="124">
         <v>44452</v>
       </c>
-      <c r="F3" s="128"/>
+      <c r="F3" s="125"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="122"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="124">
+      <c r="I4" s="121">
         <f>I5</f>
         <v>44452</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="124">
+      <c r="J4" s="122"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="122"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="121">
         <f>P5</f>
         <v>44459</v>
       </c>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="124">
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="121">
         <f>W5</f>
         <v>44466</v>
       </c>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AB4" s="125"/>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="124">
+      <c r="X4" s="122"/>
+      <c r="Y4" s="122"/>
+      <c r="Z4" s="122"/>
+      <c r="AA4" s="122"/>
+      <c r="AB4" s="122"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="121">
         <f>AD5</f>
         <v>44473</v>
       </c>
-      <c r="AE4" s="125"/>
-      <c r="AF4" s="125"/>
-      <c r="AG4" s="125"/>
-      <c r="AH4" s="125"/>
-      <c r="AI4" s="125"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="124">
+      <c r="AE4" s="122"/>
+      <c r="AF4" s="122"/>
+      <c r="AG4" s="122"/>
+      <c r="AH4" s="122"/>
+      <c r="AI4" s="122"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="121">
         <f>AK5</f>
         <v>44480</v>
       </c>
-      <c r="AL4" s="125"/>
-      <c r="AM4" s="125"/>
-      <c r="AN4" s="125"/>
-      <c r="AO4" s="125"/>
-      <c r="AP4" s="125"/>
-      <c r="AQ4" s="126"/>
-      <c r="AR4" s="124">
+      <c r="AL4" s="122"/>
+      <c r="AM4" s="122"/>
+      <c r="AN4" s="122"/>
+      <c r="AO4" s="122"/>
+      <c r="AP4" s="122"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="121">
         <f>AR5</f>
         <v>44487</v>
       </c>
-      <c r="AS4" s="125"/>
-      <c r="AT4" s="125"/>
-      <c r="AU4" s="125"/>
-      <c r="AV4" s="125"/>
-      <c r="AW4" s="125"/>
-      <c r="AX4" s="126"/>
-      <c r="AY4" s="124">
+      <c r="AS4" s="122"/>
+      <c r="AT4" s="122"/>
+      <c r="AU4" s="122"/>
+      <c r="AV4" s="122"/>
+      <c r="AW4" s="122"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="121">
         <f>AY5</f>
         <v>44494</v>
       </c>
-      <c r="AZ4" s="125"/>
-      <c r="BA4" s="125"/>
-      <c r="BB4" s="125"/>
-      <c r="BC4" s="125"/>
-      <c r="BD4" s="125"/>
-      <c r="BE4" s="126"/>
-      <c r="BF4" s="124">
+      <c r="AZ4" s="122"/>
+      <c r="BA4" s="122"/>
+      <c r="BB4" s="122"/>
+      <c r="BC4" s="122"/>
+      <c r="BD4" s="122"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="121">
         <f>BF5</f>
         <v>44501</v>
       </c>
-      <c r="BG4" s="125"/>
-      <c r="BH4" s="125"/>
-      <c r="BI4" s="125"/>
-      <c r="BJ4" s="125"/>
-      <c r="BK4" s="125"/>
-      <c r="BL4" s="126"/>
+      <c r="BG4" s="122"/>
+      <c r="BH4" s="122"/>
+      <c r="BI4" s="122"/>
+      <c r="BJ4" s="122"/>
+      <c r="BK4" s="122"/>
+      <c r="BL4" s="123"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44452</v>
@@ -2778,7 +2784,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="35">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="36">
         <f>Project_Start</f>
@@ -2861,7 +2867,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="35">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="38">
         <f>F9</f>
@@ -3184,8 +3190,8 @@
       <c r="C14" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="101">
-        <v>0.95</v>
+      <c r="D14" s="101" t="s">
+        <v>85</v>
       </c>
       <c r="E14" s="41">
         <f>F13</f>
@@ -3336,7 +3342,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="59">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E16" s="60">
         <f>E14</f>
@@ -3417,7 +3423,7 @@
         <v>54</v>
       </c>
       <c r="D17" s="62">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="63">
         <f>F16</f>
@@ -3814,7 +3820,7 @@
         <v>64</v>
       </c>
       <c r="D22" s="78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="79">
         <f>F20</f>
@@ -3894,7 +3900,9 @@
       <c r="C23" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="81"/>
+      <c r="D23" s="81">
+        <v>1</v>
+      </c>
       <c r="E23" s="82">
         <f>F22</f>
         <v>44493</v>
@@ -3973,7 +3981,9 @@
       <c r="C24" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="81"/>
+      <c r="D24" s="81" t="s">
+        <v>84</v>
+      </c>
       <c r="E24" s="82">
         <f>F23</f>
         <v>44497</v>
@@ -4052,7 +4062,9 @@
       <c r="C25" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="81"/>
+      <c r="D25" s="81">
+        <v>1</v>
+      </c>
       <c r="E25" s="82">
         <f>E22</f>
         <v>44490</v>
@@ -4204,7 +4216,9 @@
       <c r="C27" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="43"/>
+      <c r="D27" s="43">
+        <v>1</v>
+      </c>
       <c r="E27" s="44">
         <f>E25</f>
         <v>44490</v>
@@ -4283,7 +4297,9 @@
       <c r="C28" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="45">
+        <v>1</v>
+      </c>
       <c r="E28" s="46">
         <f>E27</f>
         <v>44490</v>
@@ -4433,7 +4449,9 @@
       <c r="C30" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="48"/>
+      <c r="D30" s="48">
+        <v>1</v>
+      </c>
       <c r="E30" s="49">
         <f>F28</f>
         <v>44504</v>
@@ -4512,7 +4530,9 @@
       <c r="C31" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="51"/>
+      <c r="D31" s="51">
+        <v>1</v>
+      </c>
       <c r="E31" s="52">
         <f>E30</f>
         <v>44504</v>
@@ -4593,7 +4613,9 @@
       <c r="C32" s="119" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="51"/>
+      <c r="D32" s="51">
+        <v>1</v>
+      </c>
       <c r="E32" s="52">
         <f>E30</f>
         <v>44504</v>
@@ -4672,7 +4694,9 @@
       <c r="C33" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="51"/>
+      <c r="D33" s="51">
+        <v>1</v>
+      </c>
       <c r="E33" s="52">
         <f>F32</f>
         <v>44518</v>
@@ -4745,6 +4769,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4752,11 +4781,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D11 D13:D28">
     <cfRule type="dataBar" priority="26">

</xml_diff>